<commit_message>
Nem documentation files added
</commit_message>
<xml_diff>
--- a/Design/HW/BOM/projekt.xlsx
+++ b/Design/HW/BOM/projekt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDU_OBOS_5057\Documents\Reflow oven\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDU_OBOS_5057\Documents\Reflow oven\Design\HW\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAC3D0A-F90B-469D-A327-0889CB7ADA19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5950216F-690E-4301-83F9-4B2ED0356E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5AF56432-EA0A-49C1-8877-62B3F9CD9FF4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Megnevezés</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Z3-K-1.0-1/0.315-MP-ANSI - Thermocouple, Durable PFA, 1 x 0.315mm, K, -50 °C, 350 °C, 40 ", 1 m</t>
   </si>
   <si>
-    <t>Hőelem PCB csatlakozó</t>
-  </si>
-  <si>
     <t>IM-K-PCB - Thermocouple Connector, Socket, Type K, IEC, Miniature, PCB Mount</t>
   </si>
   <si>
@@ -81,16 +78,47 @@
   </si>
   <si>
     <t>Teljesítményelektronika</t>
+  </si>
+  <si>
+    <t>MAX31855KASA+T IC</t>
+  </si>
+  <si>
+    <t>ULN2003AIPWR tranzisztor</t>
+  </si>
+  <si>
+    <t>Egyéb integrált áramkörök</t>
+  </si>
+  <si>
+    <t>Össz. Ár</t>
+  </si>
+  <si>
+    <t>Egyéb elektronikai alakatrészek</t>
+  </si>
+  <si>
+    <t>PIC24FJ256GA702-I/SO IC</t>
+  </si>
+  <si>
+    <t>PIC24FJ256GA702-I/SP IC</t>
+  </si>
+  <si>
+    <t>Plusz szállítási költségek</t>
+  </si>
+  <si>
+    <t>Farnell - FDH - GLS order 1</t>
+  </si>
+  <si>
+    <t>PICkit4 programozó</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Ft&quot;_-;\-* #,##0.00\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;Ft&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +130,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -109,9 +145,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -135,24 +177,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Pénznem" xfId="2" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -191,8 +237,8 @@
               <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -223,8 +269,8 @@
             <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -255,9 +301,9 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
                   <a:prstClr val="black">
-                    <a:alpha val="20000"/>
+                    <a:alpha val="25000"/>
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
@@ -279,9 +325,9 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
                   <a:prstClr val="black">
-                    <a:alpha val="20000"/>
+                    <a:alpha val="25000"/>
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
@@ -303,9 +349,9 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
                   <a:prstClr val="black">
-                    <a:alpha val="20000"/>
+                    <a:alpha val="25000"/>
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
@@ -327,9 +373,9 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
                   <a:prstClr val="black">
-                    <a:alpha val="20000"/>
+                    <a:alpha val="25000"/>
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
@@ -351,9 +397,9 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
                   <a:prstClr val="black">
-                    <a:alpha val="20000"/>
+                    <a:alpha val="25000"/>
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
@@ -375,9 +421,9 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
                   <a:prstClr val="black">
-                    <a:alpha val="20000"/>
+                    <a:alpha val="25000"/>
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
@@ -388,32 +434,55 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dLbls>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
-              <a:pattFill prst="pct75">
-                <a:fgClr>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:fgClr>
-                <a:bgClr>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:bgClr>
-              </a:pattFill>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
                   <a:prstClr val="black">
-                    <a:alpha val="40000"/>
+                    <a:alpha val="25000"/>
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -422,7 +491,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -434,6 +503,7 @@
                 <a:endParaRPr lang="hu-HU"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -447,9 +517,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Projekt költségek'!$A$2:$A$7</c:f>
+              <c:f>'Projekt költségek'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Sütő</c:v>
                 </c:pt>
@@ -466,17 +536,23 @@
                   <c:v>K típusú hőelem</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Hőelem PCB csatlakozó</c:v>
+                  <c:v>Egyéb elektronikai alakatrészek</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Plusz szállítási költségek</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PICkit4 programozó</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Projekt költségek'!$C$2:$C$7</c:f>
+              <c:f>'Projekt költségek'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.00\ "Ft"</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>13510</c:v>
                 </c:pt>
@@ -493,7 +569,13 @@
                   <c:v>4297.1085000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1863.471</c:v>
+                  <c:v>6325.87</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="_(&quot;Ft&quot;* #,##0.00_);_(&quot;Ft&quot;* \(#,##0.00\);_(&quot;Ft&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>1270</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,6 +587,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -524,13 +607,12 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
+            <a:alpha val="78000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:ln>
@@ -542,12 +624,12 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr rtl="0">
+          <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -571,30 +653,21 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -660,18 +733,18 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -679,125 +752,77 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="39000">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
             <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -816,34 +841,39 @@
         <a:schemeClr val="phClr"/>
       </a:solidFill>
       <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
           <a:prstClr val="black">
             <a:alpha val="20000"/>
           </a:prstClr>
         </a:outerShdw>
       </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -856,11 +886,9 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -877,10 +905,13 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
   <cs:dataPointMarkerLayout symbol="circle" size="6"/>
@@ -908,93 +939,225 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1003,172 +1166,15 @@
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-          <a:alpha val="39000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:seriesLine>
   <cs:title>
     <cs:lnRef idx="0"/>
@@ -1176,8 +1182,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
@@ -1196,6 +1202,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1205,8 +1212,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1222,13 +1229,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1238,15 +1246,10 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1270,10 +1273,10 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1598,21 +1601,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99916080-7CC7-4C0D-BC15-B61D7CFCE82A}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="87.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1623,10 +1629,16 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1638,12 +1650,22 @@
       </c>
       <c r="E2" s="1">
         <f>SUM(C:C)</f>
-        <v>81558.579500000007</v>
+        <v>107102.9785</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="6">
+        <v>290.83</v>
+      </c>
+      <c r="X2" s="1">
+        <f>SUM(V2:V500)</f>
+        <v>6325.87</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1651,8 +1673,14 @@
       <c r="C3" s="1">
         <v>16473</v>
       </c>
+      <c r="U3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="5">
+        <v>815.34</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1662,20 +1690,32 @@
       <c r="C4" s="1">
         <v>38595</v>
       </c>
+      <c r="U4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V4" s="5">
+        <v>953.77</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
         <f>1124*5+1200</f>
         <v>6820</v>
       </c>
+      <c r="U5" t="s">
+        <v>12</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1965.96</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1686,25 +1726,43 @@
         <f>3383.55*1.27</f>
         <v>4297.1085000000003</v>
       </c>
+      <c r="U6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2299.9699999999998</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1">
-        <f>1467.3*1.27</f>
-        <v>1863.471</v>
+        <f>X2</f>
+        <v>6325.87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1270</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1">
+        <v>19812</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PCB output files added
</commit_message>
<xml_diff>
--- a/Design/HW/BOM/projekt.xlsx
+++ b/Design/HW/BOM/projekt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EDU_OBOS_5057\Documents\Reflow oven\Design\HW\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5950216F-690E-4301-83F9-4B2ED0356E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581F3A31-D89A-48E5-BE76-729DF3E48B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5AF56432-EA0A-49C1-8877-62B3F9CD9FF4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="117">
   <si>
     <t>Megnevezés</t>
   </si>
@@ -101,13 +101,289 @@
     <t>PIC24FJ256GA702-I/SP IC</t>
   </si>
   <si>
-    <t>Plusz szállítási költségek</t>
-  </si>
-  <si>
-    <t>Farnell - FDH - GLS order 1</t>
-  </si>
-  <si>
     <t>PICkit4 programozó</t>
+  </si>
+  <si>
+    <t>BIO-kerámia szálas paplan 1100°C 128kg/m3</t>
+  </si>
+  <si>
+    <t>Hőszigeteleő</t>
+  </si>
+  <si>
+    <t>Szállítás</t>
+  </si>
+  <si>
+    <t>43-25-52</t>
+  </si>
+  <si>
+    <t>2 db</t>
+  </si>
+  <si>
+    <t>166.5 Ft.</t>
+  </si>
+  <si>
+    <t>43-00-81</t>
+  </si>
+  <si>
+    <t>1 db</t>
+  </si>
+  <si>
+    <t>1598 Ft.</t>
+  </si>
+  <si>
+    <t>519.2 Ft.</t>
+  </si>
+  <si>
+    <t>43-22-45</t>
+  </si>
+  <si>
+    <t>5 db</t>
+  </si>
+  <si>
+    <t>46.4 Ft.</t>
+  </si>
+  <si>
+    <t>89-23-79</t>
+  </si>
+  <si>
+    <t>76.17 Ft.</t>
+  </si>
+  <si>
+    <t>89-24-84</t>
+  </si>
+  <si>
+    <t>748.64 Ft.</t>
+  </si>
+  <si>
+    <t>87-06-44</t>
+  </si>
+  <si>
+    <t>3 db</t>
+  </si>
+  <si>
+    <t>46.7 Ft.</t>
+  </si>
+  <si>
+    <t>81-11-69</t>
+  </si>
+  <si>
+    <t>20 db</t>
+  </si>
+  <si>
+    <t>2.85 Ft.</t>
+  </si>
+  <si>
+    <t>81-11-43</t>
+  </si>
+  <si>
+    <t>10 db</t>
+  </si>
+  <si>
+    <t>4.85 Ft.</t>
+  </si>
+  <si>
+    <t>28.8 Ft.</t>
+  </si>
+  <si>
+    <t>95-03-88</t>
+  </si>
+  <si>
+    <t>12.37 Ft.</t>
+  </si>
+  <si>
+    <t>81-11-51</t>
+  </si>
+  <si>
+    <t>81-11-40</t>
+  </si>
+  <si>
+    <t>81-31-57</t>
+  </si>
+  <si>
+    <t>4.86 Ft.</t>
+  </si>
+  <si>
+    <t>82-05-98</t>
+  </si>
+  <si>
+    <t>6 db</t>
+  </si>
+  <si>
+    <t>14.59 Ft.</t>
+  </si>
+  <si>
+    <t>81-11-48</t>
+  </si>
+  <si>
+    <t>25 db</t>
+  </si>
+  <si>
+    <t>2.45 Ft.</t>
+  </si>
+  <si>
+    <t>81-27-95</t>
+  </si>
+  <si>
+    <t>2.86 Ft.</t>
+  </si>
+  <si>
+    <t>2.99 Ft.</t>
+  </si>
+  <si>
+    <t>81-00-89</t>
+  </si>
+  <si>
+    <t>2.2 Ft.</t>
+  </si>
+  <si>
+    <t>82-06-43</t>
+  </si>
+  <si>
+    <t>12 Ft.</t>
+  </si>
+  <si>
+    <t>274.1 Ft.</t>
+  </si>
+  <si>
+    <t>12-04-57</t>
+  </si>
+  <si>
+    <t>23.03 Ft.</t>
+  </si>
+  <si>
+    <t>81-11-35</t>
+  </si>
+  <si>
+    <t>82-13-76</t>
+  </si>
+  <si>
+    <t>40 db</t>
+  </si>
+  <si>
+    <t>8.05 Ft.</t>
+  </si>
+  <si>
+    <t>81-11-71</t>
+  </si>
+  <si>
+    <t>81-34-64</t>
+  </si>
+  <si>
+    <t>3.24 Ft.</t>
+  </si>
+  <si>
+    <t>12-00-62</t>
+  </si>
+  <si>
+    <t>75.43 Ft.</t>
+  </si>
+  <si>
+    <t>81-33-99</t>
+  </si>
+  <si>
+    <t>50 db</t>
+  </si>
+  <si>
+    <t>1.66 Ft.</t>
+  </si>
+  <si>
+    <t>83-01-47</t>
+  </si>
+  <si>
+    <t>3.8 Ft.</t>
+  </si>
+  <si>
+    <t>18.78 Ft.</t>
+  </si>
+  <si>
+    <t>USB-B MICRO 5P ANYA 90° MCUSB-B-S05PFHSBTH (T-T) FEMALE SMD+LOCATING PEG 90°</t>
+  </si>
+  <si>
+    <t>TÜSKESOR 64 P SOLDER TAIL PRECI 350-10-164-00-006101 (PRE) 2.54mm 5um Sn-0.25um Au 0.47/0.47mm</t>
+  </si>
+  <si>
+    <t>SORKAPOCS 9 P RM3.50 CPA3.5/9 (STE) LIFTES 1mmř 10A</t>
+  </si>
+  <si>
+    <t>SORKAPOCS 2 P RM3.50 TL001V-2P (TLM) 1qmm 6A 250V AWG24-16</t>
+  </si>
+  <si>
+    <t>NCP1117DT33RKG (ONS) FIX 3.3V 1A LDO.VOLT.REG. DPAK (LP1117,REG1117)</t>
+  </si>
+  <si>
+    <t>LM2576SX-5.0 (TI) FIX 5V 3A STEP-DOWN VOLT.REG. TO-263-5L</t>
+  </si>
+  <si>
+    <t>74HC08D (NXP) 4x2-INPUT AND-GATE SO-14</t>
+  </si>
+  <si>
+    <t>68K0 1206 5% CR-06JL7---68K 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>470R 1206 5% CR-06JL7--470R 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>3A 40V RECT.SCH. 1N5822 (YET) Vf=0.525V DO-201AD</t>
+  </si>
+  <si>
+    <t>3216 RED 631nm 120mcd HL-PC-3216S9AC (HON) W.CLEAR 3.2x1.6x0.68mm 1206 140°</t>
+  </si>
+  <si>
+    <t>2K20 1206 5% CR-06JL7---2K2 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>270R 1206 5% CR-06JL7--270R 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>220R 1206 5% WR12X221JTL 0.25W (WAL)</t>
+  </si>
+  <si>
+    <t>1uF 1206 10% 16V X7R CL31B105KOFNNNE (SAM)</t>
+  </si>
+  <si>
+    <t>1K20 1206 5% CR-06JL7---1K2 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>1K00 1206 5% WR12X102JTL 0.25W (WAL)</t>
+  </si>
+  <si>
+    <t>150R 1206 1% CR-06FL7--150R 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>11R0 1206 5% RC1206JR-0711RL 0.25W (YAG) Ł</t>
+  </si>
+  <si>
+    <t>10uF 1210 20% 10V X5R C3225X5R1A106MT000N (TDK) Ł</t>
+  </si>
+  <si>
+    <t>100uHy 12.5x12.5x 7.5mm 20% 0.125R SLF12575T-101M1R9-H (TDK) Idc=1.9A POW. SHIELDED</t>
+  </si>
+  <si>
+    <t>100uF 50V 8x11 RM 3.5 20% 105° 2000h KSC107M050S1ACG11K (TEA) LOW ESR &amp; IMP. HIGH FREQUENCY (KSC)</t>
+  </si>
+  <si>
+    <t>100R 1206 5% CR-06JL7--100R 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>100nF 1206 10% 50V X7R C1206C104K5RAC7210 (KEM)</t>
+  </si>
+  <si>
+    <t>100K 1206 5% CR-06JL7--100K 0.25W (VIK)</t>
+  </si>
+  <si>
+    <t>100K 0805 5% CR21-104-JK (ASJ)</t>
+  </si>
+  <si>
+    <t>1000uF 35V 13x20 RM5.0 20% 85° 2000h EGR108M035S1A1L200 (LUX)</t>
+  </si>
+  <si>
+    <t>0R00 1206 WR12X000PTL (WAL) Iav=2</t>
+  </si>
+  <si>
+    <t>0.1A 75V SOT-363 SWITCH 2xDUAL tr&lt;4ns BAV70S (PHI) COM.CAT. ˝A4t˝ Ł</t>
+  </si>
+  <si>
+    <t>0.1A 30V SOT-23 SCH.DUAL trr&lt;5ns BAR43SFILM (STM) ˝DA5˝ SER.</t>
   </si>
 </sst>
 </file>
@@ -118,7 +394,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Ft&quot;_-;\-* #,##0.00\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;Ft&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +435,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -182,7 +467,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -193,6 +478,21 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -284,12 +584,23 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11371647363252106"/>
+          <c:y val="7.5241951957453382E-2"/>
+          <c:w val="0.77016582827213276"/>
+          <c:h val="0.89426383062051285"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="2"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -454,6 +765,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3E94-437C-BAC9-40DCD706E94A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -475,6 +791,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3E94-437C-BAC9-40DCD706E94A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -539,10 +860,10 @@
                   <c:v>Egyéb elektronikai alakatrészek</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Plusz szállítási költségek</c:v>
+                  <c:v>PICkit4 programozó</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>PICkit4 programozó</c:v>
+                  <c:v>Hőszigeteleő</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -569,13 +890,13 @@
                   <c:v>4297.1085000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6325.87</c:v>
+                  <c:v>16569.980000000003</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="_(&quot;Ft&quot;* #,##0.00_);_(&quot;Ft&quot;* \(#,##0.00\);_(&quot;Ft&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>1270</c:v>
+                <c:pt idx="6">
+                  <c:v>19812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19812</c:v>
+                  <c:v>5813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,15 +1589,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>526676</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>481853</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>537881</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1601,13 +1922,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99916080-7CC7-4C0D-BC15-B61D7CFCE82A}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="87.42578125" bestFit="1" customWidth="1"/>
@@ -1616,9 +1937,13 @@
     <col min="21" max="21" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.5703125" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1631,14 +1956,15 @@
       <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" s="5"/>
+      <c r="AE1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1650,20 +1976,20 @@
       </c>
       <c r="E2" s="1">
         <f>SUM(C:C)</f>
-        <v>107102.9785</v>
-      </c>
-      <c r="U2" s="4" t="s">
+        <v>121890.08850000001</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="6">
+      <c r="AC2" s="6">
         <v>290.83</v>
       </c>
-      <c r="X2" s="1">
-        <f>SUM(V2:V500)</f>
-        <v>6325.87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AE2" s="1">
+        <f>SUM(AC2:AC38)</f>
+        <v>16569.980000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1673,14 +1999,14 @@
       <c r="C3" s="1">
         <v>16473</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AB3" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="5">
+      <c r="AC3" s="5">
         <v>815.34</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1690,14 +2016,14 @@
       <c r="C4" s="1">
         <v>38595</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AB4" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="5">
+      <c r="AC4" s="5">
         <v>953.77</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1708,14 +2034,14 @@
         <f>1124*5+1200</f>
         <v>6820</v>
       </c>
-      <c r="U5" t="s">
+      <c r="AB5" t="s">
         <v>12</v>
       </c>
-      <c r="V5" s="1">
+      <c r="AC5" s="5">
         <v>1965.96</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1726,42 +2052,592 @@
         <f>3383.55*1.27</f>
         <v>4297.1085000000003</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="V6" s="1">
+      <c r="AC6" s="5">
         <v>2299.9699999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1">
-        <f>X2</f>
-        <v>6325.87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <f>AE2</f>
+        <v>16569.980000000003</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>19812</v>
+      </c>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC8" s="11">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
+      <c r="B9" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>19812</v>
+        <v>5813</v>
+      </c>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC9" s="11">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10">
+        <v>16029</v>
+      </c>
+      <c r="Z10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC10" s="11">
+        <v>519.20000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z11" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC11" s="11">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC12" s="11">
+        <v>380.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC13" s="11">
+        <v>1497.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC14" s="11">
+        <v>140.11000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC15" s="11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC16" s="11">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="17" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10">
+        <v>42468</v>
+      </c>
+      <c r="Z17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC17" s="11">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC18" s="11">
+        <v>123.7</v>
+      </c>
+    </row>
+    <row r="19" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z19" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC19" s="11">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="20" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z20" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC20" s="11">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="21" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB21" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC21" s="11">
+        <v>48.6</v>
+      </c>
+    </row>
+    <row r="22" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC22" s="11">
+        <v>87.52</v>
+      </c>
+    </row>
+    <row r="23" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z23" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC23" s="11">
+        <v>61.25</v>
+      </c>
+    </row>
+    <row r="24" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z24" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB24" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC24" s="11">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="25" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10">
+        <v>29510</v>
+      </c>
+      <c r="Z25" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC25" s="11">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="26" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z26" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB26" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC26" s="11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z27" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC27" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10">
+        <v>34066</v>
+      </c>
+      <c r="Z28" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA28" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC28" s="11">
+        <v>548.20000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z29" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB29" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC29" s="11">
+        <v>230.3</v>
+      </c>
+    </row>
+    <row r="30" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC30" s="11">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="31" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z31" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB31" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC31" s="11">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z32" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA32" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC32" s="11">
+        <v>61.25</v>
+      </c>
+    </row>
+    <row r="33" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA33" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB33" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC33" s="11">
+        <v>64.8</v>
+      </c>
+    </row>
+    <row r="34" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z34" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB34" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC34" s="11">
+        <v>377.15</v>
+      </c>
+    </row>
+    <row r="35" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z35" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB35" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC35" s="11">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA36" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB36" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC36" s="11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X37" s="10"/>
+      <c r="Y37" s="10">
+        <v>30361</v>
+      </c>
+      <c r="Z37" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB37" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC37" s="11">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="38" spans="24:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC38" s="11">
+        <v>1270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>